<commit_message>
Supplementary_Data - made each column name unique.
</commit_message>
<xml_diff>
--- a/data/Supplementary_Data.xlsx
+++ b/data/Supplementary_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arnoldhk/Desktop/Research/2019CatMicrobiomes/FURTD_PLoS_Submission_Package_Reviewer_Comments/FURTD_gitlab/domestic_feline_cohort_gut_nasal_microbiomes_analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69F6165A-3D3E-4744-8254-88125F65B78E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6A7F87-2932-4B40-955D-E2D3F9CF1699}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="500" windowWidth="26660" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2420" yWindow="1240" windowWidth="26660" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animal Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="323">
   <si>
     <t>Collector</t>
   </si>
@@ -995,6 +995,9 @@
   <si>
     <t>N*</t>
   </si>
+  <si>
+    <t>Last_URI_Tx_Date</t>
+  </si>
 </sst>
 </file>
 
@@ -1954,8 +1957,8 @@
   <dimension ref="A1:BC1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A8" sqref="A8:XFD8"/>
+      <pane xSplit="1" topLeftCell="AR1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2135,7 +2138,7 @@
         <v>277</v>
       </c>
       <c r="AU1" s="25" t="s">
-        <v>293</v>
+        <v>322</v>
       </c>
       <c r="AV1" s="25" t="s">
         <v>293</v>

</xml_diff>